<commit_message>
Work plan v. 2.0.
</commit_message>
<xml_diff>
--- a/docs/workplan/CSSR4Africa_Effort.xlsx
+++ b/docs/workplan/CSSR4Africa_Effort.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/David/Documents/Research/ CSSRforAfrica/Work Plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA757B4-0561-2B49-9176-11443937BCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D6DC7A-B88A-704D-98EE-283D497D1E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="2320" windowWidth="19440" windowHeight="15940" xr2:uid="{F497874B-B98C-704D-9F0F-B6D2F108FA51}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F497874B-B98C-704D-9F0F-B6D2F108FA51}"/>
   </bookViews>
   <sheets>
-    <sheet name="Effort per Task" sheetId="1" r:id="rId1"/>
+    <sheet name="Effort by Task" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -451,7 +451,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -776,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7385A5-9CF5-0C43-83F3-F13434F46833}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -874,7 +874,7 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" ref="D5:D67" si="0">SUM(B5*C5)</f>
+        <f t="shared" ref="D5:D66" si="0">SUM(B5*C5)</f>
         <v>1.5</v>
       </c>
       <c r="E5" s="11"/>

</xml_diff>

<commit_message>
Fixed typos in effort and SoW
</commit_message>
<xml_diff>
--- a/docs/workplan/CSSR4Africa_Effort.xlsx
+++ b/docs/workplan/CSSR4Africa_Effort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/David/Documents/Research/ CSSRforAfrica/Work Plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D6DC7A-B88A-704D-98EE-283D497D1E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043970EE-80E1-3641-A367-B8F0EE21F78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F497874B-B98C-704D-9F0F-B6D2F108FA51}"/>
   </bookViews>
@@ -145,9 +145,6 @@
     <t>Task 4.2.1 ﻿People Detection and Localization</t>
   </si>
   <si>
-    <t>Task 4.2.2 ﻿Face &amp; Eye Detection and Localization}</t>
-  </si>
-  <si>
     <t>Task ﻿4.2.3 Sound Detection and Localization </t>
   </si>
   <si>
@@ -169,15 +166,9 @@
     <t xml:space="preserve">﻿Task 4.4 Use Case Feedback </t>
   </si>
   <si>
-    <t>WP5 SRobot Behaviors</t>
-  </si>
-  <si>
     <t>﻿Task 5.1 Actuator Tests</t>
   </si>
   <si>
-    <t>﻿Task 5.2 Animate Behavior Subsystem}</t>
-  </si>
-  <si>
     <t>﻿Task 5.3 Attention Subsystem</t>
   </si>
   <si>
@@ -233,6 +224,15 @@
   </si>
   <si>
     <t>Task 1.1 Rwandan Cultural Knowledge Survey</t>
+  </si>
+  <si>
+    <t>﻿Task 5.2 Animate Behavior Subsystem</t>
+  </si>
+  <si>
+    <t>WP5 Robot Behaviors</t>
+  </si>
+  <si>
+    <t>Task 4.2.2 ﻿Face &amp; Eye Detection and Localization</t>
   </si>
 </sst>
 </file>
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7385A5-9CF5-0C43-83F3-F13434F46833}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="169" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -792,7 +792,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>15</v>
@@ -801,10 +801,10 @@
         <v>1</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -823,7 +823,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B3" s="7">
         <v>3</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B4" s="7">
         <v>3</v>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="9" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B27" s="7">
         <v>6</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="7">
         <v>6</v>
@@ -1302,7 +1302,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="7">
         <v>9</v>
@@ -1323,7 +1323,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="7">
         <v>3</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="10"/>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="7">
         <v>9</v>
@@ -1376,7 +1376,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="7">
         <v>9</v>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="7">
         <v>9</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="4" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="10"/>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B37" s="7">
         <v>4</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="9" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B38" s="7">
         <v>5</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B39" s="7">
         <v>9</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="10"/>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B41" s="7">
         <v>9</v>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B42" s="7">
         <v>6</v>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B43" s="7">
         <v>6</v>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="10"/>
@@ -1589,7 +1589,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B45" s="7">
         <v>12</v>
@@ -1610,7 +1610,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B46" s="7">
         <v>6</v>
@@ -1631,7 +1631,7 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B47" s="7">
         <v>9</v>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B48" s="7">
         <v>9</v>
@@ -1673,7 +1673,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B49" s="7">
         <v>9</v>
@@ -1717,7 +1717,7 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B52" s="7">
         <v>3</v>
@@ -1738,7 +1738,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B53" s="7">
         <v>3</v>
@@ -1759,7 +1759,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B54" s="7">
         <v>3</v>

</xml_diff>

<commit_message>
Work Plan version 2.3 - Divided Task 5.5.2 into four sub-tasks to accommodate English, isiZulu, and Kinyarwanda languages
</commit_message>
<xml_diff>
--- a/docs/workplan/CSSR4Africa_Effort.xlsx
+++ b/docs/workplan/CSSR4Africa_Effort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/David/Documents/Research/ CSSRforAfrica/Work Plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043970EE-80E1-3641-A367-B8F0EE21F78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C66C60-555A-4C4B-A3C7-D5F8E1D074CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F497874B-B98C-704D-9F0F-B6D2F108FA51}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>Task Duration</t>
   </si>
@@ -233,6 +233,15 @@
   </si>
   <si>
     <t>Task 4.2.2 ﻿Face &amp; Eye Detection and Localization</t>
+  </si>
+  <si>
+    <t>﻿Task 5.5.2.1 English Text to Speech Conversion</t>
+  </si>
+  <si>
+    <t>﻿Task 5.5.2.2 isiZulu Text to Speech Conversion</t>
+  </si>
+  <si>
+    <t>﻿Task 5.5.2.3 Kinyarwanda Text to Speech Conversion</t>
   </si>
 </sst>
 </file>
@@ -774,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7385A5-9CF5-0C43-83F3-F13434F46833}">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="169" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="169" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -874,7 +883,7 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" ref="D5:D66" si="0">SUM(B5*C5)</f>
+        <f t="shared" ref="D5:D69" si="0">SUM(B5*C5)</f>
         <v>1.5</v>
       </c>
       <c r="E5" s="11"/>
@@ -1433,8 +1442,8 @@
       <c r="C36" s="10"/>
       <c r="D36" s="6"/>
       <c r="E36" s="8">
-        <f>SUM(D37:D49)</f>
-        <v>43.5</v>
+        <f>SUM(D37:D52)</f>
+        <v>49.5</v>
       </c>
       <c r="F36" s="23"/>
       <c r="G36" s="23"/>
@@ -1612,466 +1621,519 @@
       <c r="A46" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="7">
-        <v>6</v>
-      </c>
-      <c r="C46" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="D46" s="6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
+      <c r="B46" s="7"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="6"/>
       <c r="E46" s="8"/>
       <c r="F46" s="23"/>
-      <c r="G46" s="23">
-        <f>SUM($D46)</f>
-        <v>3</v>
-      </c>
+      <c r="G46" s="23"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="9" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B47" s="7">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C47" s="10">
         <v>0.5</v>
       </c>
       <c r="D47" s="6">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
+        <f t="shared" ref="D47" si="1">SUM(B47*C47)</f>
+        <v>3</v>
       </c>
       <c r="E47" s="8"/>
-      <c r="F47" s="23">
+      <c r="F47" s="23"/>
+      <c r="G47" s="23">
         <f>SUM($D47)</f>
-        <v>4.5</v>
-      </c>
-      <c r="G47" s="23"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="9" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B48" s="7">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C48" s="10">
         <v>0.5</v>
       </c>
       <c r="D48" s="6">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
+        <f t="shared" ref="D48" si="2">SUM(B48*C48)</f>
+        <v>3</v>
       </c>
       <c r="E48" s="8"/>
-      <c r="F48" s="23">
+      <c r="F48" s="23"/>
+      <c r="G48" s="23">
         <f>SUM($D48)</f>
-        <v>4.5</v>
-      </c>
-      <c r="G48" s="23"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="9" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B49" s="7">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C49" s="10">
         <v>0.5</v>
       </c>
       <c r="D49" s="6">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="23">
         <f>SUM($D49)</f>
+        <v>3</v>
+      </c>
+      <c r="G49" s="23"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="7">
+        <v>9</v>
+      </c>
+      <c r="C50" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D50" s="6">
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="G49" s="23"/>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="9"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="6"/>
       <c r="E50" s="8"/>
-      <c r="F50" s="23"/>
+      <c r="F50" s="23">
+        <f>SUM($D50)</f>
+        <v>4.5</v>
+      </c>
       <c r="G50" s="23"/>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="8">
-        <f>SUM(D52:D54)</f>
+      <c r="A51" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="7">
+        <v>9</v>
+      </c>
+      <c r="C51" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D51" s="6">
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="F51" s="23"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="23">
+        <f>SUM($D51)</f>
+        <v>4.5</v>
+      </c>
       <c r="G51" s="23"/>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52" s="7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C52" s="10">
         <v>0.5</v>
       </c>
       <c r="D52" s="6">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="E52" s="8"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23">
+      <c r="F52" s="23">
         <f>SUM($D52)</f>
-        <v>1.5</v>
-      </c>
+        <v>4.5</v>
+      </c>
+      <c r="G52" s="23"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="7">
-        <v>3</v>
-      </c>
-      <c r="C53" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="D53" s="6">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
+      <c r="A53" s="9"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="6"/>
       <c r="E53" s="8"/>
       <c r="F53" s="23"/>
-      <c r="G53" s="23">
-        <f>SUM($D53)</f>
+      <c r="G53" s="23"/>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="8">
+        <f>SUM(D55:D57)</f>
+        <v>4.5</v>
+      </c>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="7">
+        <v>3</v>
+      </c>
+      <c r="C55" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D55" s="6">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B54" s="7">
-        <v>3</v>
-      </c>
-      <c r="C54" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="D54" s="6">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="E54" s="8"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23">
-        <f>SUM($D54)</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="9"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="6"/>
       <c r="E55" s="8"/>
       <c r="F55" s="23"/>
-      <c r="G55" s="23"/>
+      <c r="G55" s="23">
+        <f>SUM($D55)</f>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="8">
-        <f>SUM(D57:D60)</f>
-        <v>6</v>
-      </c>
+      <c r="A56" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="7">
+        <v>3</v>
+      </c>
+      <c r="C56" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D56" s="6">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="E56" s="8"/>
       <c r="F56" s="23"/>
-      <c r="G56" s="23"/>
+      <c r="G56" s="23">
+        <f>SUM($D56)</f>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="9" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B57" s="7">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="C57" s="10">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="D57" s="6">
         <f t="shared" si="0"/>
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="E57" s="8"/>
-      <c r="F57" s="23">
+      <c r="F57" s="23"/>
+      <c r="G57" s="23">
         <f>SUM($D57)</f>
-        <v>1.8</v>
-      </c>
-      <c r="G57" s="23"/>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="7">
-        <v>36</v>
-      </c>
-      <c r="C58" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="D58" s="6">
-        <f t="shared" si="0"/>
-        <v>1.8</v>
-      </c>
+      <c r="A58" s="9"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="6"/>
       <c r="E58" s="8"/>
       <c r="F58" s="23"/>
-      <c r="G58" s="23">
-        <f>SUM($D58)</f>
-        <v>1.8</v>
-      </c>
+      <c r="G58" s="23"/>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" s="7">
-        <v>18</v>
-      </c>
-      <c r="C59" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="D59" s="6">
-        <f t="shared" si="0"/>
-        <v>0.9</v>
-      </c>
-      <c r="E59" s="8"/>
-      <c r="F59" s="23">
-        <f>SUM($D59)</f>
-        <v>0.9</v>
-      </c>
+      <c r="A59" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="8">
+        <f>SUM(D60:D63)</f>
+        <v>6</v>
+      </c>
+      <c r="F59" s="23"/>
       <c r="G59" s="23"/>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B60" s="7">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C60" s="10">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="D60" s="6">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="E60" s="8"/>
-      <c r="F60" s="23"/>
-      <c r="G60" s="23">
+      <c r="F60" s="23">
         <f>SUM($D60)</f>
-        <v>1.5</v>
-      </c>
+        <v>1.8</v>
+      </c>
+      <c r="G60" s="23"/>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="9"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="6"/>
+      <c r="A61" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" s="7">
+        <v>36</v>
+      </c>
+      <c r="C61" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="D61" s="6">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
       <c r="E61" s="8"/>
       <c r="F61" s="23"/>
-      <c r="G61" s="23"/>
+      <c r="G61" s="23">
+        <f>SUM($D61)</f>
+        <v>1.8</v>
+      </c>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="8">
-        <f>SUM(D63:D67)</f>
-        <v>8.4</v>
-      </c>
-      <c r="F62" s="23"/>
+      <c r="A62" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="7">
+        <v>18</v>
+      </c>
+      <c r="C62" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="D62" s="6">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="E62" s="8"/>
+      <c r="F62" s="23">
+        <f>SUM($D62)</f>
+        <v>0.9</v>
+      </c>
       <c r="G62" s="23"/>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B63" s="7">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="C63" s="10">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="D63" s="6">
         <f t="shared" si="0"/>
-        <v>1.8</v>
-      </c>
-      <c r="E63" s="11"/>
-      <c r="F63" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="E63" s="8"/>
+      <c r="F63" s="23"/>
+      <c r="G63" s="23">
         <f>SUM($D63)</f>
-        <v>1.8</v>
-      </c>
-      <c r="G63" s="23"/>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B64" s="7">
-        <v>36</v>
-      </c>
-      <c r="C64" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="D64" s="6">
-        <f t="shared" si="0"/>
-        <v>1.8</v>
-      </c>
-      <c r="E64" s="11"/>
-      <c r="F64" s="23">
-        <f>SUM($D64)</f>
-        <v>1.8</v>
-      </c>
+      <c r="A64" s="9"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="23"/>
       <c r="G64" s="23"/>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B65" s="7">
-        <v>36</v>
-      </c>
-      <c r="C65" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="D65" s="6">
-        <f t="shared" si="0"/>
-        <v>1.8</v>
-      </c>
-      <c r="E65" s="11"/>
+      <c r="A65" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="8">
+        <f>SUM(D66:D70)</f>
+        <v>8.4</v>
+      </c>
       <c r="F65" s="23"/>
-      <c r="G65" s="23">
-        <f>SUM($D65)</f>
-        <v>1.8</v>
-      </c>
+      <c r="G65" s="23"/>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B66" s="7">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C66" s="10">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="D66" s="6">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="E66" s="11"/>
-      <c r="F66" s="23"/>
-      <c r="G66" s="23">
+      <c r="F66" s="23">
         <f>SUM($D66)</f>
-        <v>1.5</v>
-      </c>
+        <v>1.8</v>
+      </c>
+      <c r="G66" s="23"/>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B67" s="7">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C67" s="10">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="D67" s="6">
-        <f>SUM(B67*C67)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>1.8</v>
       </c>
       <c r="E67" s="11"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="23">
+      <c r="F67" s="23">
         <f>SUM($D67)</f>
-        <v>1.5</v>
-      </c>
+        <v>1.8</v>
+      </c>
+      <c r="G67" s="23"/>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="9"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="6"/>
+      <c r="A68" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" s="7">
+        <v>36</v>
+      </c>
+      <c r="C68" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="D68" s="6">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
       <c r="E68" s="11"/>
       <c r="F68" s="23"/>
-      <c r="G68" s="23"/>
+      <c r="G68" s="23">
+        <f>SUM($D68)</f>
+        <v>1.8</v>
+      </c>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="12" t="s">
+      <c r="A69" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" s="7">
+        <v>3</v>
+      </c>
+      <c r="C69" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D69" s="6">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="E69" s="11"/>
+      <c r="F69" s="23"/>
+      <c r="G69" s="23">
+        <f>SUM($D69)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70" s="7">
+        <v>3</v>
+      </c>
+      <c r="C70" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D70" s="6">
+        <f>SUM(B70*C70)</f>
+        <v>1.5</v>
+      </c>
+      <c r="E70" s="11"/>
+      <c r="F70" s="23"/>
+      <c r="G70" s="23">
+        <f>SUM($D70)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="9"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="23"/>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="14">
-        <f>SUM(D2:D67)</f>
-        <v>122.85</v>
-      </c>
-      <c r="E69" s="21">
-        <f>SUM(E2:E67)</f>
-        <v>122.85000000000001</v>
-      </c>
-      <c r="F69" s="25">
-        <f>SUM(F2:F68)</f>
-        <v>81.75</v>
-      </c>
-      <c r="G69" s="25">
-        <f>SUM(G2:G68)</f>
-        <v>41.099999999999994</v>
-      </c>
-      <c r="H69" s="19"/>
-    </row>
-    <row r="70" spans="1:8">
-      <c r="A70" s="15" t="s">
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="14">
+        <f>SUM(D2:D70)</f>
+        <v>128.85</v>
+      </c>
+      <c r="E72" s="21">
+        <f>SUM(E2:E70)</f>
+        <v>128.85</v>
+      </c>
+      <c r="F72" s="25">
+        <f>SUM(F2:F71)</f>
+        <v>84.75</v>
+      </c>
+      <c r="G72" s="25">
+        <f>SUM(G2:G71)</f>
+        <v>44.099999999999994</v>
+      </c>
+      <c r="H72" s="19"/>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B70" s="16"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="17">
-        <f>SUM(D69/12)</f>
-        <v>10.237499999999999</v>
-      </c>
-      <c r="E70" s="18">
-        <f>SUM(E69/12)</f>
-        <v>10.237500000000001</v>
-      </c>
-      <c r="F70" s="18">
-        <f t="shared" ref="F70:G70" si="1">SUM(F69/12)</f>
-        <v>6.8125</v>
-      </c>
-      <c r="G70" s="18">
-        <f t="shared" si="1"/>
-        <v>3.4249999999999994</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="F71" s="26"/>
-      <c r="G71" s="26"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17">
+        <f>SUM(D72/12)</f>
+        <v>10.737499999999999</v>
+      </c>
+      <c r="E73" s="18">
+        <f>SUM(E72/12)</f>
+        <v>10.737499999999999</v>
+      </c>
+      <c r="F73" s="18">
+        <f t="shared" ref="F73:G73" si="3">SUM(F72/12)</f>
+        <v>7.0625</v>
+      </c>
+      <c r="G73" s="18">
+        <f t="shared" si="3"/>
+        <v>3.6749999999999994</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="F74" s="26"/>
+      <c r="G74" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>